<commit_message>
Well this is it
</commit_message>
<xml_diff>
--- a/Raet Recruitment 1/Self Evaluation.xlsx
+++ b/Raet Recruitment 1/Self Evaluation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\GitHub\TestAndMore\TestAndMore\Raet Recruitment 1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="18390" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -187,7 +192,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -424,6 +429,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -445,7 +453,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -723,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -781,7 +795,9 @@
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="10" t="s">
         <v>45</v>
@@ -795,7 +811,9 @@
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="9" t="s">
         <v>46</v>
@@ -811,7 +829,9 @@
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="10" t="s">
         <v>48</v>
@@ -827,7 +847,9 @@
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="10" t="s">
         <v>50</v>
@@ -843,7 +865,9 @@
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="10" t="s">
         <v>52</v>
@@ -859,7 +883,9 @@
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="10" t="s">
         <v>54</v>
@@ -875,63 +901,81 @@
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -943,63 +987,81 @@
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <v>4</v>
+      </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>5</v>
+      </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <v>3</v>
+      </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1011,35 +1073,45 @@
       <c r="A32" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3">
+        <v>5</v>
+      </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3">
+        <v>5</v>
+      </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="3"/>
+      <c r="B34" s="3">
+        <v>5</v>
+      </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="3"/>
+      <c r="B36" s="3">
+        <v>4</v>
+      </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1058,35 +1130,45 @@
       <c r="A39" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="3"/>
+      <c r="B39" s="3">
+        <v>3</v>
+      </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>4</v>
+      </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2">
+        <v>4</v>
+      </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2">
+        <v>4</v>
+      </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1098,21 +1180,27 @@
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="3"/>
+      <c r="B45" s="3">
+        <v>5</v>
+      </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <v>5</v>
+      </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>